<commit_message>
Working on implementing laws description
Working on implementing laws description
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -8276,13 +8276,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{92A357CC-3A9F-4E09-A5FC-0B5BC72FB533}" diskRevisions="1" revisionId="473" version="6">
-  <header guid="{AF02DEB3-6639-4AD6-BB0C-3B72EFE01D8B}" dateTime="2017-04-11T10:56:38" maxSheetId="4" userName="Siegel, Michael" r:id="rId15" minRId="458" maxRId="462">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
   <header guid="{5B4FCA12-9DCB-4C5E-9E67-4EC176FF6ECE}" dateTime="2018-07-10T20:20:21" maxSheetId="4" userName="Alex Bodian" r:id="rId16" minRId="463">
     <sheetIdMap count="3">
       <sheetId val="1"/>
@@ -8449,75 +8442,8 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="458" sId="1">
-    <oc r="F77" t="inlineStr">
-      <is>
-        <t>Law provides authorities with discretion in deciding whether to grant a concealed carry permit.</t>
-      </is>
-    </oc>
-    <nc r="F77" t="inlineStr">
-      <is>
-        <t>Law provides authorities with discretion in deciding whether to grant a concealed carry permit, or the law bans all concealed weapons.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="459" sId="1">
-    <oc r="F78" t="inlineStr">
-      <is>
-        <t>Law prohibits applicants from being approved for concealed carry permits unless they make a heightened showing, such as demonstrating a particular need to possess a concealed weapon.</t>
-      </is>
-    </oc>
-    <nc r="F78" t="inlineStr">
-      <is>
-        <t>Law prohibits applicants from being approved for concealed carry permits unless they make a heightened showing, such as demonstrating a particular need to possess a concealed weapon, or law bans all concealed weapons.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="460" sId="1">
-    <oc r="F79" t="inlineStr">
-      <is>
-        <t>Law requires authorities to revoke a concealed carry permit under certain circumstances.</t>
-      </is>
-    </oc>
-    <nc r="F79" t="inlineStr">
-      <is>
-        <t>Law requires authorities to revoke a concealed carry permit under certain circumstances, or law bans all concealed weapons.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="461" sId="1">
-    <oc r="F80" t="inlineStr">
-      <is>
-        <t>Law requires that individuals undergo a background check when applying for a concealed carry permit.</t>
-      </is>
-    </oc>
-    <nc r="F80" t="inlineStr">
-      <is>
-        <t>Law requires that individuals undergo a background check when applying for a concealed carry permit, or law bans all concealed weapons.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="462" sId="1">
-    <oc r="F82" t="inlineStr">
-      <is>
-        <t>Law requires individuals to undergo a background check in order to renew a concealed carry permit.</t>
-      </is>
-    </oc>
-    <nc r="F82" t="inlineStr">
-      <is>
-        <t>Law requires individuals to undergo a background check in order to renew a concealed carry permit, or law bans all concealed weapons.</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{92A357CC-3A9F-4E09-A5FC-0B5BC72FB533}" name="Alex Bodian" id="-1428285968" dateTime="2018-07-10T20:16:43"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>